<commit_message>
changes made in rfq table
</commit_message>
<xml_diff>
--- a/frontend/public/sample.xlsx
+++ b/frontend/public/sample.xlsx
@@ -1,40 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELLL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neeraj\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2466F9F8-0BCC-4FC9-B663-1BBE1300F3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9526047-44F5-4AA9-B898-D21104D8E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{22FA59C3-CEC8-4723-896F-788D87B0EAA5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Electric Actautor Sizing requirement</t>
+  </si>
   <si>
     <t>Item</t>
   </si>
@@ -45,13 +39,15 @@
     <t>Valve Tag No.</t>
   </si>
   <si>
-    <t>Valve Size (Inch)</t>
+    <t>Valve
+Size (Inch)</t>
   </si>
   <si>
     <t>Valve Rating</t>
   </si>
   <si>
-    <t>Type of Duty (On-off / Modulating)</t>
+    <t>Type of Duty 
+(On-off / Modulating)</t>
   </si>
   <si>
     <t>Raising Stem or Not</t>
@@ -60,6 +56,9 @@
     <t>Valve Torque (Nm)</t>
   </si>
   <si>
+    <t>Safety factor</t>
+  </si>
+  <si>
     <t>Valve Top Flange PCD (ISO)</t>
   </si>
   <si>
@@ -72,14 +71,17 @@
     <t>Number of Turns (for Gate and Globe valves)</t>
   </si>
   <si>
-    <t xml:space="preserve">quantity </t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Calculated Torque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,9 +93,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -105,12 +113,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF66FFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -119,28 +127,95 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -148,14 +223,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -163,6 +252,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -191,7 +285,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -203,7 +297,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -250,23 +344,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -302,23 +379,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -470,131 +530,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7838C9-93A7-4894-88C1-5BDD7B62A54B}">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.21875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" ht="54" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="N2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>